<commit_message>
update one file to one dir, startup faster, no console
</commit_message>
<xml_diff>
--- a/02.Config/config.xlsx
+++ b/02.Config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\02.Public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03.Dev\01.Project\02.AttendanceServer\02.Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAA8143-694B-4596-ADE9-E9C6D68A6D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7FB5E9-2540-4FFE-A4ED-7036BFF9612C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6354BC04-B487-417A-81BA-EC62C1F93913}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6354BC04-B487-417A-81BA-EC62C1F93913}"/>
   </bookViews>
   <sheets>
     <sheet name="ip_machines" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>192.168.1.31</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Nguyen Thi Thanh Vy</t>
+  </si>
+  <si>
+    <t>access_db</t>
+  </si>
+  <si>
+    <t>D:\OneDrive - TIQN\04.HR DB\ZK ATTENDANCE.MDB</t>
   </si>
 </sst>
 </file>
@@ -395,8 +401,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6600EFD1-F5E8-4F42-A8F3-E9FC7A212B95}" name="Table2" displayName="Table2" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9" xr:uid="{6600EFD1-F5E8-4F42-A8F3-E9FC7A212B95}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6600EFD1-F5E8-4F42-A8F3-E9FC7A212B95}" name="Table2" displayName="Table2" ref="A1:C10" totalsRowShown="0">
+  <autoFilter ref="A1:C10" xr:uid="{6600EFD1-F5E8-4F42-A8F3-E9FC7A212B95}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5A38E9EF-0B04-4D82-9003-CB80871702C0}" name="Name"/>
     <tableColumn id="2" xr3:uid="{1D4BBC50-06DD-4C6D-99BD-A980A31051FC}" name="Name2"/>
@@ -800,10 +806,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721FE71E-74BD-48D9-9C0B-CED098C2B1FB}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -906,6 +912,14 @@
         <v>27</v>
       </c>
       <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -926,7 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289C74CE-43D2-4956-8D26-E8B2BA425655}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>